<commit_message>
make dta files and function interface for prediction
</commit_message>
<xml_diff>
--- a/ProDS2/Prediction/iterasi6.xlsx
+++ b/ProDS2/Prediction/iterasi6.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -6033,7 +6033,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -7281,7 +7281,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="B583" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -7521,7 +7521,7 @@
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -7593,7 +7593,7 @@
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -7689,7 +7689,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -7857,7 +7857,7 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -7917,7 +7917,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -7941,7 +7941,7 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -8409,7 +8409,7 @@
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="B687" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -8769,7 +8769,7 @@
       </c>
       <c r="B695" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -8937,7 +8937,7 @@
       </c>
       <c r="B709" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -8961,7 +8961,7 @@
       </c>
       <c r="B711" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -9177,7 +9177,7 @@
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -9369,7 +9369,7 @@
       </c>
       <c r="B745" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -9513,7 +9513,7 @@
       </c>
       <c r="B757" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -9729,7 +9729,7 @@
       </c>
       <c r="B775" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -9837,7 +9837,7 @@
       </c>
       <c r="B784" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -10029,7 +10029,7 @@
       </c>
       <c r="B800" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -10149,7 +10149,7 @@
       </c>
       <c r="B810" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="B842" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -10617,7 +10617,7 @@
       </c>
       <c r="B849" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -10677,7 +10677,7 @@
       </c>
       <c r="B854" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
       </c>
       <c r="B872" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -10917,7 +10917,7 @@
       </c>
       <c r="B874" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -10989,7 +10989,7 @@
       </c>
       <c r="B880" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -11301,7 +11301,7 @@
       </c>
       <c r="B906" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -11349,7 +11349,7 @@
       </c>
       <c r="B910" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -11805,7 +11805,7 @@
       </c>
       <c r="B948" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -11841,7 +11841,7 @@
       </c>
       <c r="B951" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -11853,7 +11853,7 @@
       </c>
       <c r="B952" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -12537,7 +12537,7 @@
       </c>
       <c r="B1009" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -12597,7 +12597,7 @@
       </c>
       <c r="B1014" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -12705,7 +12705,7 @@
       </c>
       <c r="B1023" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -12717,7 +12717,7 @@
       </c>
       <c r="B1024" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -12741,7 +12741,7 @@
       </c>
       <c r="B1026" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -12849,7 +12849,7 @@
       </c>
       <c r="B1035" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -13029,7 +13029,7 @@
       </c>
       <c r="B1050" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -13041,7 +13041,7 @@
       </c>
       <c r="B1051" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -13173,7 +13173,7 @@
       </c>
       <c r="B1062" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -13185,7 +13185,7 @@
       </c>
       <c r="B1063" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -13257,7 +13257,7 @@
       </c>
       <c r="B1069" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -13473,7 +13473,7 @@
       </c>
       <c r="B1087" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -13557,7 +13557,7 @@
       </c>
       <c r="B1094" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -13641,7 +13641,7 @@
       </c>
       <c r="B1101" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -13677,7 +13677,7 @@
       </c>
       <c r="B1104" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -13713,7 +13713,7 @@
       </c>
       <c r="B1107" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -13761,7 +13761,7 @@
       </c>
       <c r="B1111" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -13833,7 +13833,7 @@
       </c>
       <c r="B1117" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -13905,7 +13905,7 @@
       </c>
       <c r="B1123" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -14049,7 +14049,7 @@
       </c>
       <c r="B1135" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -14169,7 +14169,7 @@
       </c>
       <c r="B1145" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -14325,7 +14325,7 @@
       </c>
       <c r="B1158" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -14337,7 +14337,7 @@
       </c>
       <c r="B1159" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -14433,7 +14433,7 @@
       </c>
       <c r="B1167" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -14613,7 +14613,7 @@
       </c>
       <c r="B1182" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -14757,7 +14757,7 @@
       </c>
       <c r="B1194" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -14949,7 +14949,7 @@
       </c>
       <c r="B1210" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -14985,7 +14985,7 @@
       </c>
       <c r="B1213" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -15093,7 +15093,7 @@
       </c>
       <c r="B1222" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -15117,7 +15117,7 @@
       </c>
       <c r="B1224" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>

</xml_diff>